<commit_message>
Finished the diagram for part 3
</commit_message>
<xml_diff>
--- a/conditional-state-table.xlsx
+++ b/conditional-state-table.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ted\ProjectCAO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\School\CompArch\ProjectCAO\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D86FCE0-75E1-4ED2-94F1-BA8A57DCA3EB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24253" windowHeight="9764"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24255" windowHeight="9765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
   <si>
     <t>rf_we</t>
   </si>
@@ -99,12 +100,66 @@
   </si>
   <si>
     <t>Condition</t>
+  </si>
+  <si>
+    <t>mm_sel</t>
+  </si>
+  <si>
+    <t>dm_we</t>
+  </si>
+  <si>
+    <t>opcode == brr  &amp;&amp;  (mm == 0000)</t>
+  </si>
+  <si>
+    <t>opcode == brr &amp;&amp;  (mm&amp;stat)</t>
+  </si>
+  <si>
+    <t>opcode == bra &amp;&amp; (mm == 0000)</t>
+  </si>
+  <si>
+    <t>opcode == bra &amp;&amp; (mm&amp;stat)</t>
+  </si>
+  <si>
+    <t>opcode == bne &amp;&amp; (mm == 0000)</t>
+  </si>
+  <si>
+    <t>opcode == bne &amp;&amp; (mm&amp;stat)</t>
+  </si>
+  <si>
+    <t>opcode == alu_op &amp;&amp; mm == 0</t>
+  </si>
+  <si>
+    <t>opcode == alu_op &amp;&amp; mm == 8</t>
+  </si>
+  <si>
+    <t>opcode == lod &amp;&amp; mm == 0</t>
+  </si>
+  <si>
+    <t>opcode == lod &amp;&amp; mm == 8</t>
+  </si>
+  <si>
+    <t>opcode == str &amp;&amp; mm == 0</t>
+  </si>
+  <si>
+    <t>opcode == str &amp;&amp; mm == 8</t>
+  </si>
+  <si>
+    <t>opcode == alu_op &amp;&amp; mm ==0</t>
+  </si>
+  <si>
+    <t>opcode == alu_op &amp;&amp; mm ==1</t>
+  </si>
+  <si>
+    <t>opcode == lod &amp;&amp; mm ==8</t>
+  </si>
+  <si>
+    <t>opcode == str</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,13 +189,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -154,20 +244,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:K16" totalsRowShown="0">
-  <autoFilter ref="A1:K16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:K16" totalsRowShown="0">
+  <autoFilter ref="A1:K16" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="State"/>
-    <tableColumn id="2" name="Condition"/>
-    <tableColumn id="3" name="rf_we"/>
-    <tableColumn id="4" name="wb_sel"/>
-    <tableColumn id="5" name="alu_op"/>
-    <tableColumn id="6" name="br_sel"/>
-    <tableColumn id="7" name="pc_rst"/>
-    <tableColumn id="8" name="pc_write"/>
-    <tableColumn id="9" name="pc_sel"/>
-    <tableColumn id="10" name="rb_sel"/>
-    <tableColumn id="11" name="ir_load"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="State"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Condition"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="rf_we"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="wb_sel"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="alu_op"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="br_sel"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pc_rst"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="pc_write"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pc_sel"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="rb_sel"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="ir_load"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{05B1EE07-1F8F-4386-8C6D-88715AF11B0E}" name="Table22" displayName="Table22" ref="A23:M53" totalsRowShown="0">
+  <autoFilter ref="A23:M53" xr:uid="{B0D30168-4B7E-4825-9E75-2C5C776ADDA9}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{A1F43FAE-92DF-4F3E-9AA2-9DF4E901B53D}" name="State"/>
+    <tableColumn id="2" xr3:uid="{DD7B1AF1-59B2-4FF4-919F-8793E7734B17}" name="Condition"/>
+    <tableColumn id="3" xr3:uid="{A2F77ABC-5383-489A-80C4-73AF47F5A79F}" name="rf_we" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{3B11A4A7-A268-4118-B1D7-59C9C4D84FC2}" name="wb_sel" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{062AB2C8-2572-4596-BECC-D5D56E3ACE81}" name="alu_op" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{37631664-56E7-4F5B-997C-BAE3E5792D3A}" name="br_sel" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{A5D88D19-E5F1-4D45-83F1-1E9748B5F246}" name="pc_rst" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{F1FFF9C3-681A-46F5-9D1B-8F1B800133EF}" name="pc_write" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{AE432B1D-F2A8-433D-854A-DC3E1C141AEB}" name="pc_sel" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{F486693F-6710-4129-A562-B78C91997947}" name="rb_sel" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{1C3B679F-07B9-414B-86B3-587A97EE5AA8}" name="ir_load" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{B292669D-9586-4EA4-9E55-2D398369B4DE}" name="mm_sel" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{60D096F7-29F9-4119-92ED-9933BCFD4117}" name="dm_we" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -469,21 +581,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -518,7 +630,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -553,7 +665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -588,7 +700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -623,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -658,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -690,7 +802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -722,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>18</v>
       </c>
@@ -754,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -786,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -821,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -853,7 +965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>21</v>
       </c>
@@ -885,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -920,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>20</v>
       </c>
@@ -952,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -987,7 +1099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>21</v>
       </c>
@@ -1019,10 +1131,1213 @@
         <v>0</v>
       </c>
     </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <v>1</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>10</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0</v>
+      </c>
+      <c r="M27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>10</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
+        <v>0</v>
+      </c>
+      <c r="M28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>10</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+      <c r="I29" s="1">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1">
+        <v>0</v>
+      </c>
+      <c r="M29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>10</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1">
+        <v>0</v>
+      </c>
+      <c r="M30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>10</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0</v>
+      </c>
+      <c r="M31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>10</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1</v>
+      </c>
+      <c r="I32" s="1">
+        <v>1</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
+        <v>0</v>
+      </c>
+      <c r="M32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>10</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
+      <c r="I33" s="1">
+        <v>1</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>10</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0</v>
+      </c>
+      <c r="M34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1">
+        <v>0</v>
+      </c>
+      <c r="M35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1">
+        <v>0</v>
+      </c>
+      <c r="M36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1">
+        <v>11</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0</v>
+      </c>
+      <c r="L37" s="1">
+        <v>0</v>
+      </c>
+      <c r="M37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <v>10</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1">
+        <v>0</v>
+      </c>
+      <c r="L38" s="1">
+        <v>1</v>
+      </c>
+      <c r="M38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <v>11</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1">
+        <v>0</v>
+      </c>
+      <c r="J39" s="1">
+        <v>0</v>
+      </c>
+      <c r="K39" s="1">
+        <v>0</v>
+      </c>
+      <c r="L39" s="1">
+        <v>0</v>
+      </c>
+      <c r="M39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1">
+        <v>10</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0</v>
+      </c>
+      <c r="K40" s="1">
+        <v>0</v>
+      </c>
+      <c r="L40" s="1">
+        <v>1</v>
+      </c>
+      <c r="M40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1">
+        <v>10</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0</v>
+      </c>
+      <c r="J41" s="1">
+        <v>0</v>
+      </c>
+      <c r="K41" s="1">
+        <v>0</v>
+      </c>
+      <c r="L41" s="1">
+        <v>0</v>
+      </c>
+      <c r="M41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0</v>
+      </c>
+      <c r="K42" s="1">
+        <v>0</v>
+      </c>
+      <c r="L42" s="1">
+        <v>0</v>
+      </c>
+      <c r="M42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1">
+        <v>11</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0</v>
+      </c>
+      <c r="I43" s="1">
+        <v>0</v>
+      </c>
+      <c r="J43" s="1">
+        <v>0</v>
+      </c>
+      <c r="K43" s="1">
+        <v>0</v>
+      </c>
+      <c r="L43" s="1">
+        <v>0</v>
+      </c>
+      <c r="M43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1">
+        <v>11</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0</v>
+      </c>
+      <c r="K44" s="1">
+        <v>0</v>
+      </c>
+      <c r="L44" s="1">
+        <v>0</v>
+      </c>
+      <c r="M44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1">
+        <v>10</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0</v>
+      </c>
+      <c r="K45" s="1">
+        <v>0</v>
+      </c>
+      <c r="L45" s="1">
+        <v>1</v>
+      </c>
+      <c r="M45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1">
+        <v>11</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0</v>
+      </c>
+      <c r="K46" s="1">
+        <v>0</v>
+      </c>
+      <c r="L46" s="1">
+        <v>0</v>
+      </c>
+      <c r="M46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1">
+        <v>10</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0</v>
+      </c>
+      <c r="I47" s="1">
+        <v>0</v>
+      </c>
+      <c r="J47" s="1">
+        <v>0</v>
+      </c>
+      <c r="K47" s="1">
+        <v>0</v>
+      </c>
+      <c r="L47" s="1">
+        <v>1</v>
+      </c>
+      <c r="M47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1">
+        <v>10</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0</v>
+      </c>
+      <c r="I48" s="1">
+        <v>0</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0</v>
+      </c>
+      <c r="K48" s="1">
+        <v>0</v>
+      </c>
+      <c r="L48" s="1">
+        <v>0</v>
+      </c>
+      <c r="M48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1">
+        <v>10</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0</v>
+      </c>
+      <c r="J49" s="1">
+        <v>0</v>
+      </c>
+      <c r="K49" s="1">
+        <v>0</v>
+      </c>
+      <c r="L49" s="1">
+        <v>0</v>
+      </c>
+      <c r="M49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <v>11</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+      <c r="H50" s="1">
+        <v>0</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0</v>
+      </c>
+      <c r="J50" s="1">
+        <v>1</v>
+      </c>
+      <c r="K50" s="1">
+        <v>0</v>
+      </c>
+      <c r="L50" s="1">
+        <v>0</v>
+      </c>
+      <c r="M50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+      <c r="E51" s="1">
+        <v>11</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0</v>
+      </c>
+      <c r="H51" s="1">
+        <v>0</v>
+      </c>
+      <c r="I51" s="1">
+        <v>0</v>
+      </c>
+      <c r="J51" s="1">
+        <v>1</v>
+      </c>
+      <c r="K51" s="1">
+        <v>0</v>
+      </c>
+      <c r="L51" s="1">
+        <v>0</v>
+      </c>
+      <c r="M51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1">
+        <v>10</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1">
+        <v>0</v>
+      </c>
+      <c r="I52" s="1">
+        <v>0</v>
+      </c>
+      <c r="J52" s="1">
+        <v>1</v>
+      </c>
+      <c r="K52" s="1">
+        <v>0</v>
+      </c>
+      <c r="L52" s="1">
+        <v>1</v>
+      </c>
+      <c r="M52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>42</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1">
+        <v>10</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0</v>
+      </c>
+      <c r="J53" s="1">
+        <v>0</v>
+      </c>
+      <c r="K53" s="1">
+        <v>0</v>
+      </c>
+      <c r="L53" s="1">
+        <v>0</v>
+      </c>
+      <c r="M53" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>